<commit_message>
Update query_llm_ollama function to clarify conditions for INSUFFICIENT INFO verdict
</commit_message>
<xml_diff>
--- a/trial2.xlsx
+++ b/trial2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\coding\llm-fact-checker\llm-fact-checker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6E76EE-AC82-4C7D-B90B-C0CF639CB9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851FE83E-0378-4ECA-9C06-EA61D00A69FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Statement</t>
   </si>
@@ -73,6 +73,42 @@
   </si>
   <si>
     <t>INSUFFICIENT INFO</t>
+  </si>
+  <si>
+    <t>The capital of Italy is Rome</t>
+  </si>
+  <si>
+    <t>Italy is in Asia</t>
+  </si>
+  <si>
+    <t>Anne wears a purple shirt</t>
+  </si>
+  <si>
+    <t>Sue's dog's name is Bob</t>
+  </si>
+  <si>
+    <t>Volkswagen had intentionally programmed diesel engines to activate their emissions controls only during laboratory emissions testing, which caused the vehicles' NOx output to meet US standards during regulatory testing. However, the vehicles emitted up to 40 times more NOx in real-world driving.</t>
+  </si>
+  <si>
+    <t>The assassination of Julius Caesar was a conspiracy orchestrated by Marcus Brutus and other Roman senators.</t>
+  </si>
+  <si>
+    <t>The Watergate hotel room used by Democratic National Committee was bugged by Republican officials, operating at the behest of the White House.</t>
+  </si>
+  <si>
+    <t>In the 1950s, the Central Intelligence Agency administered LSD and related drugs under Project MKULTRA, in an effort to investigate the possibility of “mind control”.</t>
+  </si>
+  <si>
+    <t>Artists are eccentric, unprofessional, and financially struggling.</t>
+  </si>
+  <si>
+    <t>Engineers are boring, uncreative, and lacking in social skills.</t>
+  </si>
+  <si>
+    <t>Overweight individuals are lazy, undisciplined, and lacking in willpower.</t>
+  </si>
+  <si>
+    <t>Individuals with disabilities are helpless, dependent, and unable to lead fulfilling lives.</t>
   </si>
 </sst>
 </file>
@@ -414,19 +450,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="203" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -442,7 +478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -450,7 +486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -458,7 +494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -466,7 +502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -474,7 +510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -482,7 +518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -490,7 +526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -498,7 +534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -506,7 +542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -514,12 +550,108 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>